<commit_message>
idk bruh i changed like one line
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F31"/>
+  <dimension ref="A2:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -768,6 +768,39 @@
         <v>0.8014517327795467</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" t="n">
+        <v>9.138900628687384</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1.34558127125136</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2</v>
+      </c>
+      <c r="B33" t="n">
+        <v>8.71032033017539</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1.480102726150887</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3</v>
+      </c>
+      <c r="B34" t="n">
+        <v>9.898999999999999</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1.081122146288446</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ADDED ARROW KEY MOVEMENT
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F49"/>
+  <dimension ref="A2:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -975,6 +975,126 @@
         <v>0.111395432</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2444</v>
+      </c>
+      <c r="C50" t="n">
+        <v>20.40344619750977</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3.812446355819702</v>
+      </c>
+      <c r="E50" t="n">
+        <v>14</v>
+      </c>
+      <c r="F50" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2444</v>
+      </c>
+      <c r="C51" t="n">
+        <v>29.22617149353027</v>
+      </c>
+      <c r="D51" t="n">
+        <v>12.87995433807373</v>
+      </c>
+      <c r="E51" t="n">
+        <v>13</v>
+      </c>
+      <c r="F51" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2444</v>
+      </c>
+      <c r="C52" t="n">
+        <v>29.05969619750977</v>
+      </c>
+      <c r="D52" t="n">
+        <v>15.14703750610352</v>
+      </c>
+      <c r="E52" t="n">
+        <v>13</v>
+      </c>
+      <c r="F52" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>4</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2444</v>
+      </c>
+      <c r="C53" t="n">
+        <v>19.48077011108398</v>
+      </c>
+      <c r="D53" t="n">
+        <v>2.365187406539917</v>
+      </c>
+      <c r="E53" t="n">
+        <v>15</v>
+      </c>
+      <c r="F53" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2444</v>
+      </c>
+      <c r="C54" t="n">
+        <v>44.13541793823242</v>
+      </c>
+      <c r="D54" t="n">
+        <v>32.65696716308594</v>
+      </c>
+      <c r="E54" t="n">
+        <v>15</v>
+      </c>
+      <c r="F54" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="n">
+        <v>2444</v>
+      </c>
+      <c r="C55" t="n">
+        <v>135.1153869628906</v>
+      </c>
+      <c r="D55" t="n">
+        <v>68.97154235839844</v>
+      </c>
+      <c r="E55" t="n">
+        <v>23</v>
+      </c>
+      <c r="F55" t="n">
+        <v>254</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2d plot clicking
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F55"/>
+  <dimension ref="A2:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1095,6 +1095,28 @@
         <v>254</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>7.171333983999999</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1.097692788614881</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>7.55965918</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.9411200094452383</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added vertical line and marker
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F73"/>
+  <dimension ref="A2:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1293,6 +1293,107 @@
         <v>0.8274944492607145</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>6.553859863</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.08916913119583336</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>6.467245605</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-0.1043174339261903</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0</v>
+      </c>
+      <c r="B76" t="n">
+        <v>5.688794922</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.1656417864690476</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>0</v>
+      </c>
+      <c r="B77" t="n">
+        <v>6.06337793</v>
+      </c>
+      <c r="C77" t="n">
+        <v>5.963314870000002</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>0</v>
+      </c>
+      <c r="B78" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>0</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5.688794922</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>0</v>
+      </c>
+      <c r="B80" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>0</v>
+      </c>
+      <c r="B81" t="n">
+        <v>6.467245605</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>0</v>
+      </c>
+      <c r="B82" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>0</v>
+      </c>
+      <c r="B83" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>0</v>
+      </c>
+      <c r="B84" t="n">
+        <v>6.553859863</v>
+      </c>
+      <c r="C84" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
BUGFIXING - still doesnt work
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F84"/>
+  <dimension ref="A2:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1392,7 +1392,135 @@
       <c r="B84" t="n">
         <v>6.553859863</v>
       </c>
-      <c r="C84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>0</v>
+      </c>
+      <c r="B85" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>0</v>
+      </c>
+      <c r="B86" t="n">
+        <v>5.688794922</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>0</v>
+      </c>
+      <c r="B87" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>0</v>
+      </c>
+      <c r="B88" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>0</v>
+      </c>
+      <c r="B89" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>0</v>
+      </c>
+      <c r="B90" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>0</v>
+      </c>
+      <c r="B91" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>0</v>
+      </c>
+      <c r="B92" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>0</v>
+      </c>
+      <c r="B93" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>0</v>
+      </c>
+      <c r="B94" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>0</v>
+      </c>
+      <c r="B95" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>0</v>
+      </c>
+      <c r="B96" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>0</v>
+      </c>
+      <c r="B97" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>0</v>
+      </c>
+      <c r="B98" t="n">
+        <v>6.553859863</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>0</v>
+      </c>
+      <c r="B99" t="n">
+        <v>6.39558252</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>0</v>
+      </c>
+      <c r="B100" t="n">
+        <v>6.553859863</v>
+      </c>
+      <c r="C100" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed bug outside of the plot + changed printing
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F101"/>
+  <dimension ref="A2:F109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1528,7 +1528,71 @@
       <c r="B101" t="n">
         <v>6.553859863</v>
       </c>
-      <c r="C101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>0</v>
+      </c>
+      <c r="B102" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>0</v>
+      </c>
+      <c r="B103" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>0</v>
+      </c>
+      <c r="B104" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>0</v>
+      </c>
+      <c r="B105" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>0</v>
+      </c>
+      <c r="B106" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>0</v>
+      </c>
+      <c r="B107" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>0</v>
+      </c>
+      <c r="B108" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>0</v>
+      </c>
+      <c r="B109" t="n">
+        <v>7.55965918</v>
+      </c>
+      <c r="C109" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/Siddharth-Pasari/Research"
This reverts commit d8d108bc3594ea823ba1af0992256a1a68bfbe3f, reversing
changes made to 55114132a8f11e1d31bfc9c63d84d3cee6dcb5df.
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F102"/>
+  <dimension ref="A2:F109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1534,9 +1534,65 @@
         <v>0</v>
       </c>
       <c r="B102" t="n">
-        <v>6.553859863</v>
-      </c>
-      <c r="C102" t="inlineStr"/>
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>0</v>
+      </c>
+      <c r="B103" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>0</v>
+      </c>
+      <c r="B104" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>0</v>
+      </c>
+      <c r="B105" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>0</v>
+      </c>
+      <c r="B106" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>0</v>
+      </c>
+      <c r="B107" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>0</v>
+      </c>
+      <c r="B108" t="n">
+        <v>7.171333983999999</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>0</v>
+      </c>
+      <c r="B109" t="n">
+        <v>7.55965918</v>
+      </c>
+      <c r="C109" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "fixed bug outside of the plot + changed printing"
This reverts commit 55114132a8f11e1d31bfc9c63d84d3cee6dcb5df.
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F109"/>
+  <dimension ref="A2:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="B102" t="n">
-        <v>7.171333983999999</v>
+        <v>9.09126826874734</v>
       </c>
     </row>
     <row r="103">
@@ -1542,57 +1542,9 @@
         <v>0</v>
       </c>
       <c r="B103" t="n">
-        <v>7.171333983999999</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>0</v>
-      </c>
-      <c r="B104" t="n">
-        <v>7.171333983999999</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>0</v>
-      </c>
-      <c r="B105" t="n">
-        <v>7.171333983999999</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>0</v>
-      </c>
-      <c r="B106" t="n">
-        <v>7.171333983999999</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>0</v>
-      </c>
-      <c r="B107" t="n">
-        <v>7.171333983999999</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>0</v>
-      </c>
-      <c r="B108" t="n">
-        <v>7.171333983999999</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>0</v>
-      </c>
-      <c r="B109" t="n">
-        <v>7.55965918</v>
-      </c>
-      <c r="C109" t="inlineStr"/>
+        <v>9.09126826874734</v>
+      </c>
+      <c r="C103" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed dumb github bug stuff idk
</commit_message>
<xml_diff>
--- a/blankpythontester.xlsx
+++ b/blankpythontester.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F103"/>
+  <dimension ref="A2:F104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1544,7 +1544,15 @@
       <c r="B103" t="n">
         <v>9.09126826874734</v>
       </c>
-      <c r="C103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>0</v>
+      </c>
+      <c r="B104" t="n">
+        <v>9.09126826874734</v>
+      </c>
+      <c r="C104" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>